<commit_message>
Added crucesEnDiagonal and crucesEnDiagonal methods
</commit_message>
<xml_diff>
--- a/Recursos/GridReynas.xlsx
+++ b/Recursos/GridReynas.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\carlos_28\Documents\Ceti\Ingenieria\5toPlusPlus\IA\ai-code-2020-a\Recursos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{12853C9D-8564-4EBD-9EFB-6E1C60B726A2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{845A8406-FF98-45B8-BF9E-3E4BA386F432}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{4D1392D3-5E16-495F-917E-389ADA8CF863}"/>
+    <workbookView xWindow="5490" yWindow="555" windowWidth="21600" windowHeight="11385" xr2:uid="{4D1392D3-5E16-495F-917E-389ADA8CF863}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="73">
   <si>
     <t>1</t>
   </si>
@@ -58,6 +58,198 @@
   </si>
   <si>
     <t>Y/X</t>
+  </si>
+  <si>
+    <t>0,0</t>
+  </si>
+  <si>
+    <t>1,1</t>
+  </si>
+  <si>
+    <t>2,2</t>
+  </si>
+  <si>
+    <t>3,3</t>
+  </si>
+  <si>
+    <t>4,4</t>
+  </si>
+  <si>
+    <t>5,5</t>
+  </si>
+  <si>
+    <t>6,6</t>
+  </si>
+  <si>
+    <t>7,7</t>
+  </si>
+  <si>
+    <t>0,1</t>
+  </si>
+  <si>
+    <t>0,2</t>
+  </si>
+  <si>
+    <t>0,3</t>
+  </si>
+  <si>
+    <t>0,4</t>
+  </si>
+  <si>
+    <t>0,5</t>
+  </si>
+  <si>
+    <t>0,6</t>
+  </si>
+  <si>
+    <t>0,7</t>
+  </si>
+  <si>
+    <t>1,0</t>
+  </si>
+  <si>
+    <t>1,2</t>
+  </si>
+  <si>
+    <t>1,3</t>
+  </si>
+  <si>
+    <t>1,4</t>
+  </si>
+  <si>
+    <t>1,5</t>
+  </si>
+  <si>
+    <t>1,6</t>
+  </si>
+  <si>
+    <t>1,7</t>
+  </si>
+  <si>
+    <t>2,0</t>
+  </si>
+  <si>
+    <t>2,1</t>
+  </si>
+  <si>
+    <t>2,3</t>
+  </si>
+  <si>
+    <t>2,4</t>
+  </si>
+  <si>
+    <t>2,5</t>
+  </si>
+  <si>
+    <t>2,6</t>
+  </si>
+  <si>
+    <t>2,7</t>
+  </si>
+  <si>
+    <t>3,0</t>
+  </si>
+  <si>
+    <t>3,1</t>
+  </si>
+  <si>
+    <t>3,2</t>
+  </si>
+  <si>
+    <t>3,4</t>
+  </si>
+  <si>
+    <t>3,5</t>
+  </si>
+  <si>
+    <t>3,6</t>
+  </si>
+  <si>
+    <t>3,7</t>
+  </si>
+  <si>
+    <t>4,0</t>
+  </si>
+  <si>
+    <t>4,1</t>
+  </si>
+  <si>
+    <t>4,2</t>
+  </si>
+  <si>
+    <t>4,3</t>
+  </si>
+  <si>
+    <t>4,5</t>
+  </si>
+  <si>
+    <t>4,6</t>
+  </si>
+  <si>
+    <t>4,7</t>
+  </si>
+  <si>
+    <t>5,0</t>
+  </si>
+  <si>
+    <t>5,1</t>
+  </si>
+  <si>
+    <t>5,2</t>
+  </si>
+  <si>
+    <t>5,3</t>
+  </si>
+  <si>
+    <t>5,4</t>
+  </si>
+  <si>
+    <t>5,6</t>
+  </si>
+  <si>
+    <t>5,7</t>
+  </si>
+  <si>
+    <t>6,0</t>
+  </si>
+  <si>
+    <t>6,1</t>
+  </si>
+  <si>
+    <t>6,2</t>
+  </si>
+  <si>
+    <t>6,3</t>
+  </si>
+  <si>
+    <t>6,4</t>
+  </si>
+  <si>
+    <t>6,5</t>
+  </si>
+  <si>
+    <t>6,7</t>
+  </si>
+  <si>
+    <t>7,0</t>
+  </si>
+  <si>
+    <t>7,1</t>
+  </si>
+  <si>
+    <t>7,2</t>
+  </si>
+  <si>
+    <t>7,3</t>
+  </si>
+  <si>
+    <t>7,4</t>
+  </si>
+  <si>
+    <t>7,5</t>
+  </si>
+  <si>
+    <t>7,6</t>
   </si>
 </sst>
 </file>
@@ -436,13 +628,14 @@
   <dimension ref="A1:I19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L10" sqref="L10"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="8.5703125" style="1" customWidth="1"/>
-    <col min="2" max="16384" width="11.42578125" style="1"/>
+    <col min="2" max="2" width="11.42578125" style="1" customWidth="1"/>
+    <col min="3" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
@@ -478,105 +671,233 @@
       <c r="A2" s="2">
         <v>0</v>
       </c>
-      <c r="B2" s="2"/>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
-      <c r="E2" s="2"/>
-      <c r="F2" s="2"/>
-      <c r="G2" s="2"/>
-      <c r="H2" s="2"/>
-      <c r="I2" s="2"/>
+      <c r="B2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="3" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A3" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-      <c r="E3" s="2"/>
-      <c r="F3" s="2"/>
-      <c r="G3" s="2"/>
-      <c r="H3" s="2"/>
-      <c r="I3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="4" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A4" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2"/>
-      <c r="E4" s="2"/>
-      <c r="F4" s="2"/>
-      <c r="G4" s="2"/>
-      <c r="H4" s="2"/>
-      <c r="I4" s="2"/>
+      <c r="B4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="5" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A5" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
-      <c r="G5" s="2"/>
-      <c r="H5" s="2"/>
-      <c r="I5" s="2"/>
+      <c r="B5" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="6" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A6" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="B6" s="2"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="2"/>
-      <c r="H6" s="2"/>
-      <c r="I6" s="2"/>
+      <c r="B6" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="7" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A7" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="2"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="2"/>
-      <c r="H7" s="2"/>
-      <c r="I7" s="2"/>
+      <c r="B7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>71</v>
+      </c>
     </row>
     <row r="8" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2"/>
-      <c r="C8" s="2"/>
-      <c r="D8" s="2"/>
-      <c r="E8" s="2"/>
-      <c r="F8" s="2"/>
-      <c r="G8" s="2"/>
-      <c r="H8" s="2"/>
-      <c r="I8" s="2"/>
+      <c r="B8" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="9" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A9" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="B9" s="2"/>
-      <c r="C9" s="2"/>
-      <c r="D9" s="2"/>
-      <c r="E9" s="2"/>
-      <c r="F9" s="2"/>
-      <c r="G9" s="2"/>
-      <c r="H9" s="2"/>
-      <c r="I9" s="2"/>
+      <c r="B9" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>16</v>
+      </c>
     </row>
     <row r="11" spans="1:9" ht="23.25" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">

</xml_diff>